<commit_message>
Added a TON of files.
</commit_message>
<xml_diff>
--- a/CoursePlan.xlsx
+++ b/CoursePlan.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="45" windowWidth="20730" windowHeight="10545"/>
+    <workbookView xWindow="240" yWindow="45" windowWidth="20280" windowHeight="7590"/>
   </bookViews>
   <sheets>
     <sheet name="Course List" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="88">
   <si>
     <t>Complete?</t>
   </si>
@@ -181,12 +181,6 @@
     <t>Ending Grade</t>
   </si>
   <si>
-    <t>D-</t>
-  </si>
-  <si>
-    <t>C-</t>
-  </si>
-  <si>
     <t>ECON Credit Hours</t>
   </si>
   <si>
@@ -226,9 +220,6 @@
     <t>Retake Credit Hours</t>
   </si>
   <si>
-    <t>Check</t>
-  </si>
-  <si>
     <t>Choose</t>
   </si>
   <si>
@@ -250,12 +241,6 @@
     <t>ECO100/M160</t>
   </si>
   <si>
-    <t>German</t>
-  </si>
-  <si>
-    <t>Beginning German I</t>
-  </si>
-  <si>
     <t>Credits Behind:</t>
   </si>
   <si>
@@ -287,6 +272,12 @@
   </si>
   <si>
     <t>Not Offered</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>D+</t>
   </si>
 </sst>
 </file>
@@ -513,14 +504,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="4" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="5" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="5" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="4" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -873,10 +864,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I62"/>
+  <dimension ref="A1:J65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -892,20 +883,20 @@
     <col min="9" max="9" width="20.28515625" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="20.25" thickBot="1">
-      <c r="A1" s="29" t="s">
+    <row r="1" spans="1:10" ht="20.25" thickBot="1">
+      <c r="A1" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29"/>
-      <c r="G1" s="29"/>
-      <c r="H1" s="29"/>
-      <c r="I1" s="29"/>
-    </row>
-    <row r="2" spans="1:9" ht="16.5" thickTop="1" thickBot="1">
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
+    </row>
+    <row r="2" spans="1:10" ht="16.5" thickTop="1" thickBot="1">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -934,7 +925,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:10">
       <c r="A3" s="2">
         <v>100</v>
       </c>
@@ -953,14 +944,17 @@
       <c r="F3" s="2">
         <v>4</v>
       </c>
-      <c r="H3" s="4" t="s">
+      <c r="H3" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="I3" s="4" t="s">
+      <c r="I3" s="28" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="4" spans="1:9">
+      <c r="J3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
       <c r="A4" s="2">
         <v>100</v>
       </c>
@@ -982,14 +976,17 @@
       <c r="G4" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="H4" s="4" t="s">
+      <c r="H4" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="I4" s="4" t="s">
+      <c r="I4" s="28" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="5" spans="1:9">
+      <c r="J4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
       <c r="A5" s="2">
         <v>100</v>
       </c>
@@ -1011,14 +1008,17 @@
       <c r="G5" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="H5" s="4" t="s">
+      <c r="H5" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="I5" s="4" t="s">
+      <c r="I5" s="28" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="6" spans="1:9">
+      <c r="J5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
       <c r="A6" s="2">
         <v>100</v>
       </c>
@@ -1040,14 +1040,17 @@
       <c r="G6" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="H6" s="4" t="s">
+      <c r="H6" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="I6" s="4" t="s">
+      <c r="I6" s="28" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="7" spans="1:9">
+      <c r="J6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
       <c r="A7" s="2">
         <v>0</v>
       </c>
@@ -1064,19 +1067,19 @@
         <v>0</v>
       </c>
       <c r="F7" s="2">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="G7" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="H7" s="4" t="s">
+      <c r="H7" s="28" t="s">
         <v>47</v>
       </c>
-      <c r="I7" s="4" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9">
+      <c r="I7" s="28" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
       <c r="A8" s="2">
         <v>100</v>
       </c>
@@ -1098,14 +1101,17 @@
       <c r="G8" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="H8" s="4" t="s">
+      <c r="H8" s="28" t="s">
         <v>47</v>
       </c>
-      <c r="I8" s="4" t="s">
+      <c r="I8" s="28" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="9" spans="1:9">
+      <c r="J8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
       <c r="A9" s="2">
         <v>100</v>
       </c>
@@ -1127,14 +1133,17 @@
       <c r="G9" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="H9" s="4" t="s">
+      <c r="H9" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="I9" s="4" t="s">
+      <c r="I9" s="28" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="10" spans="1:9">
+      <c r="J9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
       <c r="A10" s="2">
         <v>50</v>
       </c>
@@ -1156,14 +1165,17 @@
       <c r="G10" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="H10" s="4" t="s">
+      <c r="H10" s="28" t="s">
         <v>47</v>
       </c>
-      <c r="I10" s="4" t="s">
+      <c r="I10" s="28" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="11" spans="1:9">
+      <c r="J10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
       <c r="A11" s="2">
         <v>0</v>
       </c>
@@ -1180,19 +1192,19 @@
         <v>0</v>
       </c>
       <c r="F11" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G11" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="H11" s="4" t="s">
+      <c r="H11" s="28" t="s">
         <v>46</v>
       </c>
-      <c r="I11" s="4" t="s">
+      <c r="I11" s="28" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:10">
       <c r="A12" s="2">
         <v>0</v>
       </c>
@@ -1209,19 +1221,19 @@
         <v>0</v>
       </c>
       <c r="F12" s="2">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G12" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="H12" s="4" t="s">
+      <c r="H12" s="28" t="s">
         <v>46</v>
       </c>
-      <c r="I12" s="4" t="s">
+      <c r="I12" s="28" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:10">
       <c r="A13" s="2">
         <v>100</v>
       </c>
@@ -1243,14 +1255,17 @@
       <c r="G13" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="H13" s="4" t="s">
+      <c r="H13" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="I13" s="4" t="s">
+      <c r="I13" s="28" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" s="12" customFormat="1">
+      <c r="J13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" s="12" customFormat="1">
       <c r="A14" s="5">
         <v>100</v>
       </c>
@@ -1258,10 +1273,10 @@
         <v>6</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="E14" s="5">
         <v>100</v>
@@ -1272,14 +1287,17 @@
       <c r="G14" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="H14" s="8" t="s">
+      <c r="H14" s="28" t="s">
         <v>47</v>
       </c>
-      <c r="I14" s="8" t="s">
+      <c r="I14" s="28" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="15" spans="1:9">
+      <c r="J14" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10">
       <c r="A15" s="2">
         <v>50</v>
       </c>
@@ -1290,7 +1308,7 @@
         <v>205</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="E15" s="2">
         <v>0</v>
@@ -1301,14 +1319,17 @@
       <c r="G15" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="H15" s="4" t="s">
+      <c r="H15" s="28" t="s">
         <v>47</v>
       </c>
-      <c r="I15" s="4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9">
+      <c r="I15" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="J15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10">
       <c r="A16" s="2">
         <v>0</v>
       </c>
@@ -1319,25 +1340,25 @@
         <v>320</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="E16" s="2">
         <v>0</v>
       </c>
       <c r="F16" s="2">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="H16" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="H16" s="28" t="s">
         <v>46</v>
       </c>
-      <c r="I16" s="4" t="s">
+      <c r="I16" s="28" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="1:9">
+    <row r="17" spans="1:10">
       <c r="A17" s="2">
         <v>0</v>
       </c>
@@ -1348,25 +1369,25 @@
         <v>325</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="E17" s="2">
         <v>0</v>
       </c>
       <c r="F17" s="2">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="H17" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="H17" s="28" t="s">
         <v>46</v>
       </c>
-      <c r="I17" s="4" t="s">
+      <c r="I17" s="28" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="18" spans="1:9" s="16" customFormat="1" ht="15.75" thickBot="1">
+    <row r="18" spans="1:10" s="16" customFormat="1" ht="15.75" thickBot="1">
       <c r="A18" s="19"/>
       <c r="B18" s="20"/>
       <c r="C18" s="21"/>
@@ -1378,7 +1399,7 @@
       </c>
       <c r="F18" s="19">
         <f>SUM(F3:F14)</f>
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="G18" s="30" t="s">
         <v>52</v>
@@ -1386,13 +1407,13 @@
       <c r="H18" s="30"/>
       <c r="I18" s="20">
         <f>SUM(F3:F17)</f>
-        <v>56</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" ht="15.75" thickTop="1">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="15.75" thickTop="1">
       <c r="E19" s="10"/>
     </row>
-    <row r="20" spans="1:9" s="16" customFormat="1">
+    <row r="20" spans="1:10" s="16" customFormat="1">
       <c r="A20" s="13"/>
       <c r="B20" s="14"/>
       <c r="C20" s="15"/>
@@ -1403,20 +1424,20 @@
       <c r="H20" s="14"/>
       <c r="I20" s="14"/>
     </row>
-    <row r="21" spans="1:9" ht="20.25" thickBot="1">
-      <c r="A21" s="29" t="s">
+    <row r="21" spans="1:10" ht="20.25" thickBot="1">
+      <c r="A21" s="31" t="s">
         <v>14</v>
       </c>
-      <c r="B21" s="29"/>
-      <c r="C21" s="29"/>
-      <c r="D21" s="29"/>
-      <c r="E21" s="29"/>
-      <c r="F21" s="29"/>
-      <c r="G21" s="29"/>
-      <c r="H21" s="29"/>
-      <c r="I21" s="29"/>
-    </row>
-    <row r="22" spans="1:9" ht="16.5" thickTop="1" thickBot="1">
+      <c r="B21" s="31"/>
+      <c r="C21" s="31"/>
+      <c r="D21" s="31"/>
+      <c r="E21" s="31"/>
+      <c r="F21" s="31"/>
+      <c r="G21" s="31"/>
+      <c r="H21" s="31"/>
+      <c r="I21" s="31"/>
+    </row>
+    <row r="22" spans="1:10" ht="16.5" thickTop="1" thickBot="1">
       <c r="A22" s="1" t="s">
         <v>0</v>
       </c>
@@ -1445,7 +1466,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="23" spans="1:9">
+    <row r="23" spans="1:10">
       <c r="A23" s="2">
         <v>100</v>
       </c>
@@ -1471,7 +1492,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="24" spans="1:9">
+    <row r="24" spans="1:10">
       <c r="A24" s="2">
         <v>100</v>
       </c>
@@ -1497,7 +1518,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="25" spans="1:9">
+    <row r="25" spans="1:10">
       <c r="A25" s="2">
         <v>100</v>
       </c>
@@ -1526,7 +1547,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="26" spans="1:9">
+    <row r="26" spans="1:10">
       <c r="A26" s="2">
         <v>100</v>
       </c>
@@ -1554,8 +1575,11 @@
       <c r="I26" s="4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="27" spans="1:9">
+      <c r="J26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10">
       <c r="A27" s="2">
         <v>100</v>
       </c>
@@ -1563,10 +1587,10 @@
         <v>38</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="E27" s="2">
         <v>0</v>
@@ -1575,7 +1599,7 @@
         <v>4</v>
       </c>
       <c r="G27" s="4" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="H27" s="4" t="s">
         <v>47</v>
@@ -1584,7 +1608,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="28" spans="1:9">
+    <row r="28" spans="1:10">
       <c r="A28" s="2">
         <v>50</v>
       </c>
@@ -1595,7 +1619,7 @@
         <v>202</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="E28" s="2">
         <v>0</v>
@@ -1607,10 +1631,10 @@
         <v>47</v>
       </c>
       <c r="I28" s="4" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10">
       <c r="A29" s="24">
         <v>100</v>
       </c>
@@ -1632,7 +1656,7 @@
       </c>
       <c r="F29" s="24">
         <f>$F35</f>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="G29" s="25"/>
       <c r="H29" s="25" t="str">
@@ -1644,12 +1668,12 @@
         <v>Spring</v>
       </c>
     </row>
-    <row r="30" spans="1:9" s="16" customFormat="1" ht="15.75" thickBot="1">
+    <row r="30" spans="1:10" s="16" customFormat="1" ht="15.75" thickBot="1">
       <c r="A30" s="19"/>
       <c r="B30" s="20"/>
       <c r="C30" s="21"/>
       <c r="D30" s="21" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E30" s="22" t="s">
         <v>45</v>
@@ -1664,10 +1688,10 @@
       <c r="H30" s="30"/>
       <c r="I30" s="20">
         <f>SUM(I18,F23:F28)</f>
-        <v>80</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" s="16" customFormat="1" ht="15.75" thickTop="1">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" s="16" customFormat="1" ht="15.75" thickTop="1">
       <c r="A31" s="13"/>
       <c r="B31" s="14"/>
       <c r="C31" s="15"/>
@@ -1678,7 +1702,7 @@
       <c r="H31" s="14"/>
       <c r="I31" s="14"/>
     </row>
-    <row r="32" spans="1:9" s="16" customFormat="1">
+    <row r="32" spans="1:10" s="16" customFormat="1">
       <c r="A32" s="13"/>
       <c r="B32" s="14"/>
       <c r="C32" s="15"/>
@@ -1689,20 +1713,20 @@
       <c r="H32" s="14"/>
       <c r="I32" s="14"/>
     </row>
-    <row r="33" spans="1:9" ht="20.25" thickBot="1">
-      <c r="A33" s="29" t="s">
+    <row r="33" spans="1:10" ht="20.25" thickBot="1">
+      <c r="A33" s="31" t="s">
         <v>28</v>
       </c>
-      <c r="B33" s="29"/>
-      <c r="C33" s="29"/>
-      <c r="D33" s="29"/>
-      <c r="E33" s="29"/>
-      <c r="F33" s="29"/>
-      <c r="G33" s="29"/>
-      <c r="H33" s="29"/>
-      <c r="I33" s="29"/>
-    </row>
-    <row r="34" spans="1:9" ht="16.5" thickTop="1" thickBot="1">
+      <c r="B33" s="31"/>
+      <c r="C33" s="31"/>
+      <c r="D33" s="31"/>
+      <c r="E33" s="31"/>
+      <c r="F33" s="31"/>
+      <c r="G33" s="31"/>
+      <c r="H33" s="31"/>
+      <c r="I33" s="31"/>
+    </row>
+    <row r="34" spans="1:10" ht="16.5" thickTop="1" thickBot="1">
       <c r="A34" s="1" t="s">
         <v>0</v>
       </c>
@@ -1731,7 +1755,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="35" spans="1:9">
+    <row r="35" spans="1:10">
       <c r="A35" s="2">
         <v>100</v>
       </c>
@@ -1748,7 +1772,7 @@
         <v>0</v>
       </c>
       <c r="F35" s="2">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="H35" s="4" t="s">
         <v>13</v>
@@ -1757,7 +1781,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="36" spans="1:9" s="16" customFormat="1" ht="15.75" thickBot="1">
+    <row r="36" spans="1:10" s="16" customFormat="1" ht="15.75" thickBot="1">
       <c r="A36" s="19"/>
       <c r="B36" s="20"/>
       <c r="C36" s="21"/>
@@ -1769,7 +1793,7 @@
       </c>
       <c r="F36" s="19">
         <f>SUM(F35:F35)</f>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="G36" s="30" t="s">
         <v>52</v>
@@ -1777,24 +1801,24 @@
       <c r="H36" s="30"/>
       <c r="I36" s="20">
         <f>SUM(I30,F35:F35)</f>
-        <v>84</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" ht="15.75" thickTop="1"/>
-    <row r="40" spans="1:9" ht="20.25" thickBot="1">
-      <c r="A40" s="29" t="s">
-        <v>68</v>
-      </c>
-      <c r="B40" s="29"/>
-      <c r="C40" s="29"/>
-      <c r="D40" s="29"/>
-      <c r="E40" s="29"/>
-      <c r="F40" s="29"/>
-      <c r="G40" s="29"/>
-      <c r="H40" s="29"/>
-      <c r="I40" s="29"/>
-    </row>
-    <row r="41" spans="1:9" ht="16.5" thickTop="1" thickBot="1">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" ht="15.75" thickTop="1"/>
+    <row r="40" spans="1:10" ht="20.25" thickBot="1">
+      <c r="A40" s="31" t="s">
+        <v>66</v>
+      </c>
+      <c r="B40" s="31"/>
+      <c r="C40" s="31"/>
+      <c r="D40" s="31"/>
+      <c r="E40" s="31"/>
+      <c r="F40" s="31"/>
+      <c r="G40" s="31"/>
+      <c r="H40" s="31"/>
+      <c r="I40" s="31"/>
+    </row>
+    <row r="41" spans="1:10" ht="16.5" thickTop="1" thickBot="1">
       <c r="A41" s="1" t="s">
         <v>0</v>
       </c>
@@ -1823,18 +1847,18 @@
         <v>8</v>
       </c>
     </row>
-    <row r="42" spans="1:9">
+    <row r="42" spans="1:10">
       <c r="A42" s="2">
         <v>100</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C42" s="3">
         <v>101</v>
       </c>
       <c r="D42" s="4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E42" s="2">
         <v>0</v>
@@ -1848,19 +1872,22 @@
       <c r="I42" s="4" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="43" spans="1:9">
+      <c r="J42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10">
       <c r="A43" s="2">
         <v>100</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C43" s="3">
         <v>102</v>
       </c>
       <c r="D43" s="4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E43" s="2">
         <v>0</v>
@@ -1869,7 +1896,7 @@
         <v>4</v>
       </c>
       <c r="G43" s="4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="H43" s="4" t="s">
         <v>10</v>
@@ -1877,19 +1904,22 @@
       <c r="I43" s="4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="44" spans="1:9">
+      <c r="J43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10">
       <c r="A44" s="2">
         <v>100</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C44" s="3">
         <v>171</v>
       </c>
       <c r="D44" s="4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E44" s="2">
         <v>0</v>
@@ -1904,44 +1934,29 @@
         <v>11</v>
       </c>
     </row>
-    <row r="45" spans="1:9">
+    <row r="45" spans="1:10">
       <c r="A45" s="2">
         <v>0</v>
       </c>
-      <c r="B45" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="C45" s="3">
-        <v>110</v>
-      </c>
-      <c r="D45" s="4" t="s">
-        <v>79</v>
-      </c>
       <c r="E45" s="2">
         <v>0</v>
       </c>
       <c r="F45" s="2">
-        <v>4</v>
-      </c>
-      <c r="H45" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="I45" s="4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10">
       <c r="A46" s="2">
         <v>100</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="C46" s="3">
         <v>105</v>
       </c>
       <c r="D46" s="4" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="E46" s="2">
         <v>0</v>
@@ -1956,44 +1971,44 @@
         <v>11</v>
       </c>
     </row>
-    <row r="47" spans="1:9">
+    <row r="47" spans="1:10">
       <c r="A47" s="2">
         <v>50</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="C47" s="3">
         <v>250</v>
       </c>
       <c r="D47" s="4" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E47" s="2">
         <v>0</v>
       </c>
       <c r="F47" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H47" s="4" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="I47" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="48" spans="1:9">
+    <row r="48" spans="1:10">
       <c r="A48" s="2">
         <v>50</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="C48" s="3">
         <v>380</v>
       </c>
       <c r="D48" s="4" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="E48" s="2">
         <v>100</v>
@@ -2002,175 +2017,192 @@
         <v>4</v>
       </c>
       <c r="H48" s="4" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="I48" s="4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="49" spans="1:9">
+      <c r="J48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10">
       <c r="A49" s="2">
         <v>50</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="C49" s="3">
         <v>500</v>
       </c>
       <c r="D49" s="4" t="s">
-        <v>85</v>
+        <v>80</v>
+      </c>
+      <c r="E49" s="2">
+        <v>0</v>
       </c>
       <c r="F49" s="2">
         <v>1</v>
       </c>
       <c r="H49" s="4" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="I49" s="4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="50" spans="1:9">
+      <c r="J49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10">
       <c r="A50" s="2">
         <v>0</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>72</v>
+        <v>78</v>
+      </c>
+      <c r="C50" s="3">
+        <v>501</v>
       </c>
       <c r="D50" s="4" t="s">
-        <v>71</v>
+        <v>80</v>
+      </c>
+      <c r="E50" s="2">
+        <v>0</v>
       </c>
       <c r="F50" s="2">
-        <v>4</v>
+        <v>0</v>
+      </c>
+      <c r="G50" s="4">
+        <v>500</v>
       </c>
       <c r="H50" s="4" t="s">
         <v>46</v>
       </c>
       <c r="I50" s="4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="51" spans="1:9">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10">
       <c r="A51" s="2">
         <v>0</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>72</v>
+        <v>78</v>
+      </c>
+      <c r="C51" s="3">
+        <v>510</v>
       </c>
       <c r="D51" s="4" t="s">
-        <v>71</v>
+        <v>80</v>
+      </c>
+      <c r="E51" s="2">
+        <v>0</v>
       </c>
       <c r="F51" s="2">
-        <v>4</v>
+        <v>0</v>
+      </c>
+      <c r="G51" s="4">
+        <v>500</v>
       </c>
       <c r="H51" s="4" t="s">
         <v>46</v>
       </c>
       <c r="I51" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10">
+      <c r="A52" s="2">
+        <v>0</v>
+      </c>
+      <c r="B52" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="D52" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="E52" s="2">
+        <v>0</v>
+      </c>
+      <c r="F52" s="2">
+        <v>0</v>
+      </c>
+      <c r="H52" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="I52" s="4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="52" spans="1:9" ht="15.75" thickBot="1">
-      <c r="A52" s="19"/>
-      <c r="B52" s="20"/>
-      <c r="C52" s="21"/>
-      <c r="D52" s="21" t="s">
-        <v>59</v>
-      </c>
-      <c r="E52" s="22" t="s">
+    <row r="53" spans="1:10" ht="15.75" thickBot="1">
+      <c r="A53" s="19"/>
+      <c r="B53" s="20"/>
+      <c r="C53" s="21"/>
+      <c r="D53" s="21" t="s">
+        <v>57</v>
+      </c>
+      <c r="E53" s="22" t="s">
         <v>45</v>
       </c>
-      <c r="F52" s="19">
-        <f>SUM(F42:F51)</f>
-        <v>33</v>
-      </c>
-      <c r="G52" s="30" t="s">
+      <c r="F53" s="19">
+        <f>SUM(F42:F52)</f>
+        <v>19</v>
+      </c>
+      <c r="G53" s="30" t="s">
         <v>52</v>
       </c>
-      <c r="H52" s="30"/>
-      <c r="I52" s="20">
-        <f>SUM(I36,F42:F51)</f>
-        <v>117</v>
-      </c>
-    </row>
-    <row r="53" spans="1:9" ht="15.75" thickTop="1"/>
-    <row r="55" spans="1:9" ht="20.25" thickBot="1">
-      <c r="A55" s="29" t="s">
+      <c r="H53" s="30"/>
+      <c r="I53" s="20">
+        <f>SUM(I36,F42:F52)</f>
+        <v>83</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" ht="15.75" thickTop="1"/>
+    <row r="56" spans="1:10" ht="20.25" thickBot="1">
+      <c r="A56" s="31" t="s">
         <v>53</v>
       </c>
-      <c r="B55" s="29"/>
-      <c r="C55" s="29"/>
-      <c r="D55" s="29"/>
-      <c r="E55" s="29"/>
-      <c r="F55" s="29"/>
-      <c r="G55" s="29"/>
-      <c r="H55" s="29"/>
-      <c r="I55" s="29"/>
-    </row>
-    <row r="56" spans="1:9" ht="16.5" thickTop="1" thickBot="1">
-      <c r="A56" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B56" s="6" t="s">
+      <c r="B56" s="31"/>
+      <c r="C56" s="31"/>
+      <c r="D56" s="31"/>
+      <c r="E56" s="31"/>
+      <c r="F56" s="31"/>
+      <c r="G56" s="31"/>
+      <c r="H56" s="31"/>
+      <c r="I56" s="31"/>
+    </row>
+    <row r="57" spans="1:10" ht="16.5" thickTop="1" thickBot="1">
+      <c r="A57" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B57" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="C56" s="7" t="s">
+      <c r="C57" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="D56" s="6" t="s">
+      <c r="D57" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="E56" s="1" t="s">
+      <c r="E57" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="F56" s="1" t="s">
+      <c r="F57" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="G56" s="6" t="s">
+      <c r="G57" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="H56" s="9" t="s">
+      <c r="H57" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="I56" s="9" t="s">
+      <c r="I57" s="9" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="57" spans="1:9">
-      <c r="A57" s="2">
-        <v>100</v>
-      </c>
-      <c r="B57" s="4" t="str">
-        <f>$B35</f>
-        <v>Mathematics</v>
-      </c>
-      <c r="C57" s="3">
-        <f>$C35</f>
-        <v>160</v>
-      </c>
-      <c r="D57" s="4" t="str">
-        <f>$D35</f>
-        <v>Calculus I</v>
-      </c>
-      <c r="E57" s="2">
-        <f>$E35</f>
-        <v>0</v>
-      </c>
-      <c r="F57" s="2">
-        <v>0</v>
-      </c>
-      <c r="G57" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="H57" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="I57" s="4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="58" spans="1:9">
+    <row r="58" spans="1:10">
       <c r="A58" s="2">
         <v>100</v>
       </c>
@@ -2191,103 +2223,146 @@
         <v>0</v>
       </c>
       <c r="F58" s="2">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="G58" s="4" t="s">
-        <v>56</v>
+        <v>86</v>
       </c>
       <c r="H58" s="4" t="s">
         <v>10</v>
       </c>
       <c r="I58" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10">
+      <c r="A59" s="2">
+        <v>100</v>
+      </c>
+      <c r="B59" s="4" t="str">
+        <f>$B35</f>
+        <v>Mathematics</v>
+      </c>
+      <c r="C59" s="3">
+        <f>$C35</f>
+        <v>160</v>
+      </c>
+      <c r="D59" s="4" t="str">
+        <f>$D35</f>
+        <v>Calculus I</v>
+      </c>
+      <c r="E59" s="2">
+        <f>$E35</f>
+        <v>0</v>
+      </c>
+      <c r="F59" s="2">
+        <v>0</v>
+      </c>
+      <c r="G59" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="H59" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I59" s="4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="59" spans="1:9" ht="15.75" thickBot="1">
-      <c r="A59" s="19"/>
-      <c r="B59" s="20"/>
-      <c r="C59" s="21"/>
-      <c r="D59" s="21" t="s">
-        <v>69</v>
-      </c>
-      <c r="E59" s="22" t="s">
+    <row r="60" spans="1:10">
+      <c r="G60" s="4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10">
+      <c r="G61" s="4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" ht="15.75" thickBot="1">
+      <c r="A62" s="19"/>
+      <c r="B62" s="20"/>
+      <c r="C62" s="21"/>
+      <c r="D62" s="21" t="s">
+        <v>67</v>
+      </c>
+      <c r="E62" s="22" t="s">
         <v>45</v>
       </c>
-      <c r="F59" s="19">
-        <f>SUM(F57:F58)</f>
-        <v>4</v>
-      </c>
-      <c r="G59" s="30" t="s">
+      <c r="F62" s="19">
+        <f>SUM(F58:F61)</f>
+        <v>0</v>
+      </c>
+      <c r="G62" s="30" t="s">
         <v>52</v>
       </c>
-      <c r="H59" s="30"/>
-      <c r="I59" s="20">
-        <f>SUM(I52,F57:F58)</f>
-        <v>121</v>
-      </c>
-    </row>
-    <row r="60" spans="1:9" ht="15.75" thickTop="1">
-      <c r="A60"/>
-      <c r="B60"/>
-      <c r="C60"/>
-      <c r="D60"/>
-      <c r="E60"/>
-      <c r="F60"/>
-      <c r="G60" s="31" t="s">
-        <v>67</v>
-      </c>
-      <c r="H60" s="31"/>
-      <c r="I60" s="27">
-        <f>I59</f>
-        <v>121</v>
-      </c>
-    </row>
-    <row r="61" spans="1:9">
-      <c r="A61"/>
-      <c r="B61"/>
-      <c r="C61"/>
-      <c r="D61"/>
-      <c r="E61"/>
-      <c r="F61"/>
-      <c r="G61" s="31" t="s">
-        <v>66</v>
-      </c>
-      <c r="H61" s="31"/>
-      <c r="I61" s="27">
+      <c r="H62" s="30"/>
+      <c r="I62" s="20">
+        <f>SUM(I53,F58:F61)</f>
+        <v>83</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" ht="15.75" thickTop="1">
+      <c r="A63"/>
+      <c r="B63"/>
+      <c r="C63"/>
+      <c r="D63"/>
+      <c r="E63"/>
+      <c r="F63"/>
+      <c r="G63" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="H63" s="29"/>
+      <c r="I63" s="27">
+        <f>I62</f>
+        <v>83</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10">
+      <c r="A64"/>
+      <c r="B64"/>
+      <c r="C64"/>
+      <c r="D64"/>
+      <c r="E64"/>
+      <c r="F64"/>
+      <c r="G64" s="29" t="s">
+        <v>64</v>
+      </c>
+      <c r="H64" s="29"/>
+      <c r="I64" s="27">
         <v>128</v>
       </c>
     </row>
-    <row r="62" spans="1:9">
-      <c r="A62"/>
-      <c r="B62"/>
-      <c r="C62"/>
-      <c r="D62"/>
-      <c r="E62"/>
-      <c r="F62"/>
-      <c r="G62" s="31" t="s">
-        <v>80</v>
-      </c>
-      <c r="H62" s="31"/>
-      <c r="I62" s="27">
-        <f>I61-I60</f>
-        <v>7</v>
+    <row r="65" spans="1:9">
+      <c r="A65"/>
+      <c r="B65"/>
+      <c r="C65"/>
+      <c r="D65"/>
+      <c r="E65"/>
+      <c r="F65"/>
+      <c r="G65" s="29" t="s">
+        <v>75</v>
+      </c>
+      <c r="H65" s="29"/>
+      <c r="I65" s="27">
+        <f>I64-I63</f>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="G60:H60"/>
-    <mergeCell ref="G61:H61"/>
-    <mergeCell ref="G62:H62"/>
-    <mergeCell ref="G36:H36"/>
-    <mergeCell ref="G59:H59"/>
     <mergeCell ref="A1:I1"/>
     <mergeCell ref="A21:I21"/>
     <mergeCell ref="A33:I33"/>
-    <mergeCell ref="A55:I55"/>
+    <mergeCell ref="A56:I56"/>
     <mergeCell ref="A40:I40"/>
-    <mergeCell ref="G52:H52"/>
+    <mergeCell ref="G53:H53"/>
     <mergeCell ref="G18:H18"/>
     <mergeCell ref="G30:H30"/>
+    <mergeCell ref="G63:H63"/>
+    <mergeCell ref="G64:H64"/>
+    <mergeCell ref="G65:H65"/>
+    <mergeCell ref="G36:H36"/>
+    <mergeCell ref="G62:H62"/>
   </mergeCells>
   <conditionalFormatting sqref="A1">
     <cfRule type="iconSet" priority="35">
@@ -2314,7 +2389,7 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A63:A1048576 A1:A59 G60:G62">
+  <conditionalFormatting sqref="A66:A1048576 G63:G65 A62 A1:A60">
     <cfRule type="iconSet" priority="25">
       <iconSet iconSet="3Symbols" showValue="0">
         <cfvo type="percent" val="0"/>
@@ -2365,7 +2440,7 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E61:E1048576 E34:E54 E2:E20 E22:E32 E56:E59">
+  <conditionalFormatting sqref="E64:E1048576 E34:E55 E2:E20 E22:E32 E62 E57:E60">
     <cfRule type="iconSet" priority="24">
       <iconSet iconSet="3Symbols2" showValue="0">
         <cfvo type="percent" val="0"/>
@@ -2374,7 +2449,7 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F61:F1048576 F56:F58 F53:F54 F22:F29 F34:F35 F2:F17 F37:F51">
+  <conditionalFormatting sqref="F64:F1048576 F37:F52 F54:F55 F22:F29 F34:F35 F2:F17 F57:F60">
     <cfRule type="dataBar" priority="23">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -2383,7 +2458,7 @@
       </dataBar>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H61:H1048576 H56:H59 H34:H54 H2:H17 H22:H32">
+  <conditionalFormatting sqref="H64:H1048576 H22:H32 H34:H55 H2:H17 H62 H57:H60">
     <cfRule type="containsText" dxfId="5" priority="19" operator="containsText" text="Senior">
       <formula>NOT(ISERROR(SEARCH("Senior",H2)))</formula>
     </cfRule>
@@ -2397,7 +2472,7 @@
       <formula>NOT(ISERROR(SEARCH("Freshman",H2)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I56:I1048576 I34:I54 I2:I20 I22:I32">
+  <conditionalFormatting sqref="I22:I32 I34:I55 I2:I20 I62:I1048576 I57:I60">
     <cfRule type="containsText" dxfId="1" priority="17" operator="containsText" text="Spring">
       <formula>NOT(ISERROR(SEARCH("Spring",I2)))</formula>
     </cfRule>

</xml_diff>